<commit_message>
User doc language update
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_user/screenshots.xlsx
+++ b/lisha1.00/doc_user/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-4180" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-4660" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2959,6 +2959,765 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>355</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>358</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Image 49"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5930900" y="67792600"/>
+          <a:ext cx="7454900" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>356</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>357</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Rectangle 50"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7353300" y="67894200"/>
+          <a:ext cx="876300" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>362</xdr:row>
+      <xdr:rowOff>50690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>378</xdr:row>
+      <xdr:rowOff>12699</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Image 51"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1282700" y="69011690"/>
+          <a:ext cx="8356600" cy="3010009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>376</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>378</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Rectangle 52"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438400" y="71767700"/>
+          <a:ext cx="5981700" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>381</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>397</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Image 53"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2540000" y="72732900"/>
+          <a:ext cx="8331200" cy="2946400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>384</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>385</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Rectangle 54"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3708400" y="73202800"/>
+          <a:ext cx="5981700" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>395</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>397</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="Rectangle 55"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3708400" y="75412600"/>
+          <a:ext cx="5981700" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>403</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>421</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Image 56"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1714500" y="76936600"/>
+          <a:ext cx="8991600" cy="3403600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>406</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>409</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="Ellipse 58"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3416300" y="77343000"/>
+          <a:ext cx="673100" cy="635000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>419</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>422</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="Ellipse 59"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3403600" y="79857600"/>
+          <a:ext cx="673100" cy="635000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>419</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>424</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Image 60"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12547600" y="79997300"/>
+          <a:ext cx="1841500" cy="825500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>418</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>760429</xdr:colOff>
+      <xdr:row>421</xdr:row>
+      <xdr:rowOff>144142</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Flèche vers la gauche 61"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18413163">
+          <a:off x="13528844" y="79905056"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>421</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>423</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="Ellipse 62"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13411200" y="80251300"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3291,8 +4050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="O351" sqref="O351"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A407" workbookViewId="0">
+      <selection activeCell="R412" sqref="R412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
calendar return issue and documentation
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_user/screenshots.xlsx
+++ b/lisha1.00/doc_user/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-4660" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-3200" yWindow="0" windowWidth="22380" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -3718,6 +3718,3101 @@
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>432</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>447</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Image 57"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3175000" y="82334100"/>
+          <a:ext cx="2794000" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>437</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>438</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="Rectangle 63"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3378200" y="83337400"/>
+          <a:ext cx="1638300" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>435</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>441</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="Image 64"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8686800" y="83007200"/>
+          <a:ext cx="2120900" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>437</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>439</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Ellipse 65"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9131300" y="83375500"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>434</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>633429</xdr:colOff>
+      <xdr:row>438</xdr:row>
+      <xdr:rowOff>4442</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Flèche vers la gauche 66"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18413163">
+          <a:off x="9274344" y="83003856"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>456</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>461</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="Image 67"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3733800" y="86944200"/>
+          <a:ext cx="1295400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>456</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>458</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Ellipse 68"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3848100" y="87045800"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>453</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>303229</xdr:colOff>
+      <xdr:row>457</xdr:row>
+      <xdr:rowOff>55242</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Flèche vers la gauche 69"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18413163">
+          <a:off x="3991144" y="86674156"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>450</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>465</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="Image 70"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8547100" y="85750400"/>
+          <a:ext cx="2463800" cy="2959100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>463</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>464</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="Rectangle 71"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9004300" y="88214200"/>
+          <a:ext cx="1701800" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>79544</xdr:colOff>
+      <xdr:row>463</xdr:row>
+      <xdr:rowOff>72856</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>769786</xdr:colOff>
+      <xdr:row>464</xdr:row>
+      <xdr:rowOff>71285</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="Flèche vers la gauche 72"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10811044" y="88274356"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>452</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>453</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="Ellipse 73"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8915400" y="86118700"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>467</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>491</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="77" name="Image 76"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="939800" y="89065100"/>
+          <a:ext cx="6578600" cy="4597400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>467</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>469</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="Ellipse 77"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="977900" y="89141300"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>472</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>487</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="Rectangle 78"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3873500" y="90081100"/>
+          <a:ext cx="1587500" cy="2768600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>368301</xdr:colOff>
+      <xdr:row>466</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>233043</xdr:colOff>
+      <xdr:row>467</xdr:row>
+      <xdr:rowOff>74629</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="Flèche vers la gauche 79"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="1193801" y="88849200"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>495</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>515</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="81" name="Image 80"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514600" y="94297500"/>
+          <a:ext cx="6299200" cy="3962400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>518</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>532</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="82" name="Image 81"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9093200" y="98767900"/>
+          <a:ext cx="2133600" cy="2603500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>520</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>522</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="Rectangle 82"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9385300" y="99225100"/>
+          <a:ext cx="1739900" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>518</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>194942</xdr:colOff>
+      <xdr:row>519</xdr:row>
+      <xdr:rowOff>176229</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="84" name="Flèche vers la gauche 83"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="11061700" y="98856800"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>527</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>532</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Image 74"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2044700" y="100545900"/>
+          <a:ext cx="2921000" cy="889000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>529</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>531</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="Rectangle 84"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476500" y="100914200"/>
+          <a:ext cx="292100" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>539</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>544</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Image 75"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1943100" y="102768400"/>
+          <a:ext cx="7518400" cy="1016000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>541</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>542</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="Rectangle 85"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2286000" y="103149400"/>
+          <a:ext cx="292100" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>541</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>542</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="87" name="Rectangle 86"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5245100" y="103162100"/>
+          <a:ext cx="292100" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>541</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>542</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="88" name="Rectangle 87"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8178800" y="103162100"/>
+          <a:ext cx="292100" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>184746</xdr:colOff>
+      <xdr:row>549</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>482599</xdr:colOff>
+      <xdr:row>587</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="90" name="Image 89"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2661246" y="104673400"/>
+          <a:ext cx="5250853" cy="7213600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>552</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>587</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="91" name="Rectangle 90"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4927600" y="105232200"/>
+          <a:ext cx="2540000" cy="6654800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>564</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>566</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="Flèche vers la gauche 91"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7531100" y="107518200"/>
+          <a:ext cx="1181100" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>593</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>612</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="93" name="Image 92"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3086100" y="113042700"/>
+          <a:ext cx="4089400" cy="3556000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>594</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>597</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="94" name="Rectangle 93"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3505200" y="113284000"/>
+          <a:ext cx="2895600" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>595</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>597</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="95" name="Flèche vers la gauche 94"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6489700" y="113385600"/>
+          <a:ext cx="1181100" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>601</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>615</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="96" name="Image 95"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8978900" y="114515900"/>
+          <a:ext cx="3733800" cy="2768600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>603</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>605</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="97" name="Rectangle 96"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10287000" y="115023900"/>
+          <a:ext cx="1346200" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>597</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>603</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="98" name="Flèche vers la gauche 97"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="10375900" y="114185700"/>
+          <a:ext cx="1181100" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>621</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>628</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="99" name="Image 98"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1003300" y="118427500"/>
+          <a:ext cx="9601200" cy="1282700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>637</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>649</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="89" name="Image 88"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3086100" y="121462800"/>
+          <a:ext cx="2362200" cy="2184400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>638</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>639</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="100" name="Ellipse 99"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3390900" y="121577100"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>636</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>220342</xdr:colOff>
+      <xdr:row>637</xdr:row>
+      <xdr:rowOff>87329</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="Flèche vers la gauche 100"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="3657600" y="121246900"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>639</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>647</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="102" name="Image 101"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6769100" y="121742200"/>
+          <a:ext cx="1955800" cy="1663700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>638</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>647</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="103" name="Image 102"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10299700" y="121678700"/>
+          <a:ext cx="1778000" cy="1612900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>639</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>641</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="104" name="Ellipse 103"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7137400" y="121831100"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>637</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>664842</xdr:colOff>
+      <xdr:row>638</xdr:row>
+      <xdr:rowOff>150829</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="105" name="Flèche vers la gauche 104"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="7404100" y="121500900"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>736601</xdr:colOff>
+      <xdr:row>639</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>641</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="106" name="Ellipse 105"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10642601" y="121831100"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>177801</xdr:colOff>
+      <xdr:row>637</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>42543</xdr:colOff>
+      <xdr:row>638</xdr:row>
+      <xdr:rowOff>150829</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="107" name="Flèche vers la gauche 106"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="10909301" y="121500900"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>653</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>659</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="108" name="Image 107"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6629400" y="124434600"/>
+          <a:ext cx="1600200" cy="1168400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>653</xdr:row>
+      <xdr:rowOff>50799</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>812801</xdr:colOff>
+      <xdr:row>654</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="109" name="Ellipse 108"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7061201" y="124447299"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>723901</xdr:colOff>
+      <xdr:row>651</xdr:row>
+      <xdr:rowOff>101599</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>588643</xdr:colOff>
+      <xdr:row>652</xdr:row>
+      <xdr:rowOff>100028</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="110" name="Flèche vers la gauche 109"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="7327901" y="124117099"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>662</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>669</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="111" name="Image 110"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514600" y="126136400"/>
+          <a:ext cx="2146300" cy="1447800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>663</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>622299</xdr:colOff>
+      <xdr:row>664</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="112" name="Ellipse 111"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2743199" y="126314200"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>661</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>398141</xdr:colOff>
+      <xdr:row>662</xdr:row>
+      <xdr:rowOff>61929</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="113" name="Flèche vers la gauche 112"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="3009899" y="125984000"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4050,8 +7145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A407" workbookViewId="0">
-      <selection activeCell="R412" sqref="R412"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A642" workbookViewId="0">
+      <selection activeCell="G668" sqref="G668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Add shortcut CTRL +F11 for quick help
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_user/screenshots.xlsx
+++ b/lisha1.00/doc_user/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-3200" yWindow="0" windowWidth="22380" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23000" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -6774,6 +6774,1376 @@
       <xdr:spPr>
         <a:xfrm rot="19058695">
           <a:off x="3009899" y="125984000"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>666</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>677</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="114" name="Image 113"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9550400" y="126911100"/>
+          <a:ext cx="2057400" cy="2146300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>668</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>670</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="115" name="Ellipse 114"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10236200" y="127368300"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>666</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>461642</xdr:colOff>
+      <xdr:row>667</xdr:row>
+      <xdr:rowOff>163529</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="116" name="Flèche vers la gauche 115"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="10502900" y="127038100"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>677</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>683</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="117" name="Image 116"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6350000" y="129032000"/>
+          <a:ext cx="1473200" cy="1257300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>677</xdr:row>
+      <xdr:rowOff>165101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>431799</xdr:colOff>
+      <xdr:row>679</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="118" name="Ellipse 117"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6680199" y="129133601"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>676</xdr:row>
+      <xdr:rowOff>25401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>207641</xdr:colOff>
+      <xdr:row>677</xdr:row>
+      <xdr:rowOff>23830</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="Flèche vers la gauche 118"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="6946899" y="128803401"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>691</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>699</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="121" name="Image 120"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2387600" y="131737100"/>
+          <a:ext cx="4508500" cy="1511300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>691</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>817242</xdr:colOff>
+      <xdr:row>692</xdr:row>
+      <xdr:rowOff>11129</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="123" name="Flèche vers la gauche 122"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="4254500" y="131648200"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>482601</xdr:colOff>
+      <xdr:row>691</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>347343</xdr:colOff>
+      <xdr:row>692</xdr:row>
+      <xdr:rowOff>11129</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="125" name="Flèche vers la gauche 124"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="2959101" y="131648200"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>690</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>741042</xdr:colOff>
+      <xdr:row>691</xdr:row>
+      <xdr:rowOff>176229</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="126" name="Flèche vers la gauche 125"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="5829300" y="131622800"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>692</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>698</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="128" name="Image 127"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9918700" y="131876800"/>
+          <a:ext cx="1663700" cy="1181100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>692</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>220342</xdr:colOff>
+      <xdr:row>693</xdr:row>
+      <xdr:rowOff>11129</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="129" name="Flèche vers la gauche 128"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="11087100" y="131838700"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>710</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>725</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="120" name="Image 119"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2298700" y="135318500"/>
+          <a:ext cx="3149600" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>711</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>779142</xdr:colOff>
+      <xdr:row>712</xdr:row>
+      <xdr:rowOff>87329</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="127" name="Flèche vers la gauche 126"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="4216400" y="135534400"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>704</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>719</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="122" name="Image 121"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7353300" y="134124700"/>
+          <a:ext cx="2362200" cy="3009900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>707</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>718</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="130" name="Rectangle 129"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7772400" y="134810500"/>
+          <a:ext cx="1752600" cy="2070100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>705</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>245742</xdr:colOff>
+      <xdr:row>706</xdr:row>
+      <xdr:rowOff>150829</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="131" name="Flèche vers la gauche 130"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="9461500" y="134454900"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>726</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>741</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="124" name="Image 123"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7721600" y="138379200"/>
+          <a:ext cx="3390900" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>774698</xdr:colOff>
+      <xdr:row>731</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>639440</xdr:colOff>
+      <xdr:row>732</xdr:row>
+      <xdr:rowOff>188928</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="132" name="Flèche vers la gauche 131"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="10680698" y="139445999"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>733</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>735</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="133" name="Rectangle 132"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9664700" y="139788900"/>
+          <a:ext cx="1092200" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>730</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>158964</xdr:colOff>
+      <xdr:row>756</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="134" name="Image 133"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2222500" y="139204700"/>
+          <a:ext cx="2063964" cy="4876800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>733</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>756</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="135" name="Rectangle 134"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2374900" y="139700000"/>
+          <a:ext cx="1511300" cy="4356100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>731</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>398143</xdr:colOff>
+      <xdr:row>732</xdr:row>
+      <xdr:rowOff>87329</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="136" name="Flèche vers la gauche 135"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="3835401" y="139344400"/>
           <a:ext cx="690242" cy="188929"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
@@ -7145,8 +8515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A642" workbookViewId="0">
-      <selection activeCell="G668" sqref="G668"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A724" workbookViewId="0">
+      <selection activeCell="I743" sqref="I743"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
javascript optimization and documentation
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_user/screenshots.xlsx
+++ b/lisha1.00/doc_user/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23000" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="-4920" yWindow="40" windowWidth="23000" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -64,20 +64,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>797</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>803</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 7"/>
+        <xdr:cNvPr id="152" name="Image 151"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -90,8 +90,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8839200" y="9359900"/>
-          <a:ext cx="1816100" cy="1193800"/>
+          <a:off x="3098800" y="151930100"/>
+          <a:ext cx="3263900" cy="1130300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -109,20 +109,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>95946</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>165099</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPr id="8" name="Image 7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -135,8 +135,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1346200" y="1048446"/>
-          <a:ext cx="10261600" cy="6165153"/>
+          <a:off x="8839200" y="9359900"/>
+          <a:ext cx="1816100" cy="1193800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -152,203 +152,22 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95946</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1257300" y="1295400"/>
-          <a:ext cx="10490200" cy="203200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9080500" y="1041400"/>
-          <a:ext cx="914400" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Connecteur droit avec flèche 3"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="10058400" y="1244600"/>
-          <a:ext cx="495300" cy="279400"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 4"/>
+        <xdr:cNvPr id="2" name="Image 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -361,8 +180,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4610100" y="8991600"/>
-          <a:ext cx="2247900" cy="850900"/>
+          <a:off x="1346200" y="1048446"/>
+          <a:ext cx="10261600" cy="6165153"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -380,56 +199,50 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>357393</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>25699</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>203925</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>117839</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Flèche vers la gauche 8"/>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="19732440">
-          <a:off x="6135893" y="8979199"/>
-          <a:ext cx="672032" cy="282640"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
+        <a:xfrm>
+          <a:off x="1257300" y="1295400"/>
+          <a:ext cx="10490200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -446,27 +259,27 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>227532</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>54041</xdr:rowOff>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Flèche vers la gauche 9"/>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="19732440">
-          <a:off x="9461500" y="9677401"/>
-          <a:ext cx="672032" cy="282640"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
+        <a:xfrm>
+          <a:off x="9080500" y="1041400"/>
+          <a:ext cx="914400" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
@@ -508,6 +321,238 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Connecteur droit avec flèche 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10058400" y="1244600"/>
+          <a:ext cx="495300" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4610100" y="8991600"/>
+          <a:ext cx="2247900" cy="850900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>357393</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>25699</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>203925</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>117839</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Flèche vers la gauche 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19732440">
+          <a:off x="6135893" y="8979199"/>
+          <a:ext cx="672032" cy="282640"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>227532</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>54041</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Flèche vers la gauche 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19732440">
+          <a:off x="9461500" y="9677401"/>
+          <a:ext cx="672032" cy="282640"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -529,7 +574,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1204,7 +1249,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1525,51 +1570,6 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2882900" y="20815300"/>
-          <a:ext cx="5321300" cy="1041400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="43000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Image 21"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
@@ -1577,8 +1577,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3733800" y="23291800"/>
-          <a:ext cx="8382000" cy="2984500"/>
+          <a:off x="2882900" y="20815300"/>
+          <a:ext cx="5321300" cy="1041400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1596,20 +1596,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>156</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Image 27"/>
+        <xdr:cNvPr id="22" name="Image 21"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1622,8 +1622,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5219700" y="28994100"/>
-          <a:ext cx="2120900" cy="812800"/>
+          <a:off x="3733800" y="23291800"/>
+          <a:ext cx="8382000" cy="2984500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1639,87 +1639,22 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>93940</xdr:colOff>
-      <xdr:row>151</xdr:row>
-      <xdr:rowOff>133135</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>241893</xdr:colOff>
-      <xdr:row>153</xdr:row>
-      <xdr:rowOff>40529</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="Flèche vers la gauche 28"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="19368541">
-          <a:off x="6697940" y="28898635"/>
-          <a:ext cx="973453" cy="288394"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>157</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Image 29"/>
+        <xdr:cNvPr id="28" name="Image 27"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1732,8 +1667,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9080500" y="29908500"/>
-          <a:ext cx="1511300" cy="749300"/>
+          <a:off x="5219700" y="28994100"/>
+          <a:ext cx="2120900" cy="812800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1751,25 +1686,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>249553</xdr:colOff>
-      <xdr:row>156</xdr:row>
-      <xdr:rowOff>186794</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>93940</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>133135</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>241893</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>40529</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="Flèche vers la gauche 30"/>
+        <xdr:cNvPr id="29" name="Flèche vers la gauche 28"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="19368541">
-          <a:off x="10007600" y="29616400"/>
+          <a:off x="6697940" y="28898635"/>
           <a:ext cx="973453" cy="288394"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
@@ -1816,6 +1751,116 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Image 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9080500" y="29908500"/>
+          <a:ext cx="1511300" cy="749300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>249553</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>186794</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Flèche vers la gauche 30"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19368541">
+          <a:off x="10007600" y="29616400"/>
+          <a:ext cx="973453" cy="288394"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
       <xdr:row>165</xdr:row>
@@ -1835,7 +1880,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2089,7 +2134,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2212,7 +2257,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2329,7 +2374,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2511,7 +2556,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2628,7 +2673,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2810,7 +2855,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2985,7 +3030,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3095,7 +3140,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3205,7 +3250,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3387,7 +3432,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3569,7 +3614,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3744,7 +3789,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3861,7 +3906,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4043,7 +4088,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4225,7 +4270,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4479,7 +4524,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4733,7 +4778,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4778,7 +4823,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4960,7 +5005,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5077,7 +5122,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5338,7 +5383,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5520,7 +5565,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5702,7 +5747,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5884,7 +5929,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5929,7 +5974,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6111,7 +6156,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6156,7 +6201,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6475,7 +6520,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6657,7 +6702,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6839,7 +6884,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7021,7 +7066,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7203,7 +7248,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7438,116 +7483,6 @@
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="128" name="Image 127"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9918700" y="131876800"/>
-          <a:ext cx="1663700" cy="1181100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="43000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>692</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>220342</xdr:colOff>
-      <xdr:row>693</xdr:row>
-      <xdr:rowOff>11129</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="129" name="Flèche vers la gauche 128"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="19058695">
-          <a:off x="11087100" y="131838700"/>
-          <a:ext cx="690242" cy="188929"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>710</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>725</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="120" name="Image 119"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7560,8 +7495,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2298700" y="135318500"/>
-          <a:ext cx="3149600" cy="2895600"/>
+          <a:off x="9918700" y="131876800"/>
+          <a:ext cx="1663700" cy="1181100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7579,25 +7514,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>711</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>779142</xdr:colOff>
-      <xdr:row>712</xdr:row>
-      <xdr:rowOff>87329</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>692</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>220342</xdr:colOff>
+      <xdr:row>693</xdr:row>
+      <xdr:rowOff>11129</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="127" name="Flèche vers la gauche 126"/>
+        <xdr:cNvPr id="129" name="Flèche vers la gauche 128"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="19058695">
-          <a:off x="4216400" y="135534400"/>
+          <a:off x="11087100" y="131838700"/>
           <a:ext cx="690242" cy="188929"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
@@ -7644,6 +7579,116 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>710</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>725</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="120" name="Image 119"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2298700" y="135318500"/>
+          <a:ext cx="3149600" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>711</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>779142</xdr:colOff>
+      <xdr:row>712</xdr:row>
+      <xdr:rowOff>87329</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="127" name="Flèche vers la gauche 126"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="4216400" y="135534400"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>749300</xdr:colOff>
       <xdr:row>704</xdr:row>
@@ -7663,7 +7708,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7845,7 +7890,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8027,7 +8072,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8183,6 +8228,756 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>754</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>766</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="137" name="Image 136"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6362700" y="143637000"/>
+          <a:ext cx="4432300" cy="2324100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>657057</xdr:colOff>
+      <xdr:row>756</xdr:row>
+      <xdr:rowOff>41443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>20486</xdr:colOff>
+      <xdr:row>759</xdr:row>
+      <xdr:rowOff>160185</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="138" name="Flèche vers la gauche 137"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="13995619">
+          <a:off x="6184901" y="144310099"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>756</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>760</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="141" name="Connecteur en arc 140"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7035800" y="144018000"/>
+          <a:ext cx="2197100" cy="787400"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>759</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>761</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="143" name="Ellipse 142"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6680200" y="144678400"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>755</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>756</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="144" name="Rectangle 143"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9245600" y="143840200"/>
+          <a:ext cx="1155700" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>771</xdr:row>
+      <xdr:rowOff>136464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>789</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="139" name="Image 138"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2463800" y="147011964"/>
+          <a:ext cx="7277100" cy="3406835"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>785</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>789</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="145" name="Ellipse 144"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3035300" y="149707600"/>
+          <a:ext cx="647700" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>775</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>787</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="146" name="Connecteur en arc 145"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="145" idx="6"/>
+          <a:endCxn id="147" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3683000" y="147713700"/>
+          <a:ext cx="4483100" cy="2298700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>774</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>776</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="147" name="Ellipse 146"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8166100" y="147548600"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>798</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>800</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="151" name="Rectangle 150"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4546600" y="152146000"/>
+          <a:ext cx="863600" cy="292100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>799</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>805</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="153" name="Image 152"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8255000" y="152209500"/>
+          <a:ext cx="2552700" cy="1193800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>799</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>801</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="154" name="Rectangle 153"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8483600" y="152374600"/>
+          <a:ext cx="1828800" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="lgDashDot"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -8515,8 +9310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A724" workbookViewId="0">
-      <selection activeCell="I743" sqref="I743"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A783" workbookViewId="0">
+      <selection activeCell="O799" sqref="O799"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Keep navigation in documentation and CSS bug fix
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_user/screenshots.xlsx
+++ b/lisha1.00/doc_user/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-4920" yWindow="40" windowWidth="23000" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22120" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -8941,6 +8941,417 @@
             <a:srgbClr val="FF0000"/>
           </a:solidFill>
           <a:prstDash val="lgDashDot"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>810</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>823</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="140" name="Image 139"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="154381200"/>
+          <a:ext cx="4686300" cy="2565400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>815</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>831</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="142" name="Image 141"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6515100" y="155257500"/>
+          <a:ext cx="6057900" cy="3048000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>832</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>843</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="148" name="Image 147"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="158635700"/>
+          <a:ext cx="4330700" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>821</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>830</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="155" name="Rectangle 154"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6375400" y="156540200"/>
+          <a:ext cx="444500" cy="1587500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>815</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>817</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="156" name="Rectangle 155"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8229600" y="155397200"/>
+          <a:ext cx="609600" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>817</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>821</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="157" name="Connecteur en arc 156"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="155" idx="0"/>
+          <a:endCxn id="156" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="7146925" y="155152725"/>
+          <a:ext cx="838200" cy="1936750"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>833</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>835</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="158" name="Rectangle 157"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="158775400"/>
+          <a:ext cx="914400" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
           <a:tailEnd type="arrow"/>
         </a:ln>
         <a:effectLst>
@@ -9310,8 +9721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A783" workbookViewId="0">
-      <selection activeCell="O799" sqref="O799"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A808" workbookViewId="0">
+      <selection activeCell="N809" sqref="N809"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Limited column option in update mode Extension of documentation Number format localization
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_user/screenshots.xlsx
+++ b/lisha1.00/doc_user/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22120" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="17160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -64,20 +64,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>797</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>803</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>850</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>855</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="152" name="Image 151"/>
+        <xdr:cNvPr id="150" name="Image 149"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -90,8 +90,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3098800" y="151930100"/>
-          <a:ext cx="3263900" cy="1130300"/>
+          <a:off x="6807200" y="161950400"/>
+          <a:ext cx="3086100" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -109,20 +109,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>797</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>803</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 7"/>
+        <xdr:cNvPr id="152" name="Image 151"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -135,8 +135,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8839200" y="9359900"/>
-          <a:ext cx="1816100" cy="1193800"/>
+          <a:off x="3098800" y="151930100"/>
+          <a:ext cx="3263900" cy="1130300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -154,20 +154,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>95946</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>165099</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPr id="8" name="Image 7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -180,8 +180,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1346200" y="1048446"/>
-          <a:ext cx="10261600" cy="6165153"/>
+          <a:off x="8839200" y="9359900"/>
+          <a:ext cx="1816100" cy="1193800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -197,203 +197,22 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95946</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1257300" y="1295400"/>
-          <a:ext cx="10490200" cy="203200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9080500" y="1041400"/>
-          <a:ext cx="914400" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Connecteur droit avec flèche 3"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="10058400" y="1244600"/>
-          <a:ext cx="495300" cy="279400"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 4"/>
+        <xdr:cNvPr id="2" name="Image 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -406,8 +225,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4610100" y="8991600"/>
-          <a:ext cx="2247900" cy="850900"/>
+          <a:off x="1346200" y="1048446"/>
+          <a:ext cx="10261600" cy="6165153"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -425,56 +244,50 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>357393</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>25699</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>203925</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>117839</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Flèche vers la gauche 8"/>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="19732440">
-          <a:off x="6135893" y="8979199"/>
-          <a:ext cx="672032" cy="282640"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
+        <a:xfrm>
+          <a:off x="1257300" y="1295400"/>
+          <a:ext cx="10490200" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -491,27 +304,27 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>227532</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>54041</xdr:rowOff>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Flèche vers la gauche 9"/>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="19732440">
-          <a:off x="9461500" y="9677401"/>
-          <a:ext cx="672032" cy="282640"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
+        <a:xfrm>
+          <a:off x="9080500" y="1041400"/>
+          <a:ext cx="914400" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
@@ -553,6 +366,238 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Connecteur droit avec flèche 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10058400" y="1244600"/>
+          <a:ext cx="495300" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4610100" y="8991600"/>
+          <a:ext cx="2247900" cy="850900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>357393</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>25699</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>203925</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>117839</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Flèche vers la gauche 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19732440">
+          <a:off x="6135893" y="8979199"/>
+          <a:ext cx="672032" cy="282640"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>227532</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>54041</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Flèche vers la gauche 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19732440">
+          <a:off x="9461500" y="9677401"/>
+          <a:ext cx="672032" cy="282640"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -574,7 +619,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1249,7 +1294,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1570,51 +1615,6 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2882900" y="20815300"/>
-          <a:ext cx="5321300" cy="1041400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="43000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Image 21"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
@@ -1622,8 +1622,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3733800" y="23291800"/>
-          <a:ext cx="8382000" cy="2984500"/>
+          <a:off x="2882900" y="20815300"/>
+          <a:ext cx="5321300" cy="1041400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1641,20 +1641,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>156</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Image 27"/>
+        <xdr:cNvPr id="22" name="Image 21"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1667,8 +1667,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5219700" y="28994100"/>
-          <a:ext cx="2120900" cy="812800"/>
+          <a:off x="3733800" y="23291800"/>
+          <a:ext cx="8382000" cy="2984500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1684,87 +1684,22 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>93940</xdr:colOff>
-      <xdr:row>151</xdr:row>
-      <xdr:rowOff>133135</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>241893</xdr:colOff>
-      <xdr:row>153</xdr:row>
-      <xdr:rowOff>40529</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="Flèche vers la gauche 28"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="19368541">
-          <a:off x="6697940" y="28898635"/>
-          <a:ext cx="973453" cy="288394"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>157</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Image 29"/>
+        <xdr:cNvPr id="28" name="Image 27"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1777,8 +1712,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9080500" y="29908500"/>
-          <a:ext cx="1511300" cy="749300"/>
+          <a:off x="5219700" y="28994100"/>
+          <a:ext cx="2120900" cy="812800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1796,25 +1731,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>249553</xdr:colOff>
-      <xdr:row>156</xdr:row>
-      <xdr:rowOff>186794</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>93940</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>133135</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>241893</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>40529</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="Flèche vers la gauche 30"/>
+        <xdr:cNvPr id="29" name="Flèche vers la gauche 28"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="19368541">
-          <a:off x="10007600" y="29616400"/>
+          <a:off x="6697940" y="28898635"/>
           <a:ext cx="973453" cy="288394"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
@@ -1861,6 +1796,116 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Image 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9080500" y="29908500"/>
+          <a:ext cx="1511300" cy="749300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>249553</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>186794</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Flèche vers la gauche 30"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19368541">
+          <a:off x="10007600" y="29616400"/>
+          <a:ext cx="973453" cy="288394"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
       <xdr:row>165</xdr:row>
@@ -1880,7 +1925,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2134,7 +2179,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2257,7 +2302,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2374,7 +2419,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2556,7 +2601,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2673,7 +2718,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2855,7 +2900,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3030,7 +3075,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3140,7 +3185,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3250,7 +3295,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3432,7 +3477,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3614,7 +3659,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3789,7 +3834,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3906,7 +3951,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4088,7 +4133,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4270,7 +4315,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4524,7 +4569,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4778,7 +4823,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4823,7 +4868,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5005,7 +5050,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5122,7 +5167,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5383,7 +5428,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5565,7 +5610,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5747,7 +5792,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5929,7 +5974,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5974,7 +6019,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6156,7 +6201,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6201,7 +6246,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6520,7 +6565,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6702,7 +6747,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6884,7 +6929,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7066,7 +7111,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7248,7 +7293,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7483,116 +7528,6 @@
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="128" name="Image 127"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9918700" y="131876800"/>
-          <a:ext cx="1663700" cy="1181100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="43000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>692</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>220342</xdr:colOff>
-      <xdr:row>693</xdr:row>
-      <xdr:rowOff>11129</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="129" name="Flèche vers la gauche 128"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="19058695">
-          <a:off x="11087100" y="131838700"/>
-          <a:ext cx="690242" cy="188929"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>710</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>725</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="120" name="Image 119"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7605,8 +7540,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2298700" y="135318500"/>
-          <a:ext cx="3149600" cy="2895600"/>
+          <a:off x="9918700" y="131876800"/>
+          <a:ext cx="1663700" cy="1181100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7624,25 +7559,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>711</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>779142</xdr:colOff>
-      <xdr:row>712</xdr:row>
-      <xdr:rowOff>87329</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>692</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>220342</xdr:colOff>
+      <xdr:row>693</xdr:row>
+      <xdr:rowOff>11129</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="127" name="Flèche vers la gauche 126"/>
+        <xdr:cNvPr id="129" name="Flèche vers la gauche 128"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="19058695">
-          <a:off x="4216400" y="135534400"/>
+          <a:off x="11087100" y="131838700"/>
           <a:ext cx="690242" cy="188929"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
@@ -7689,6 +7624,116 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>710</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>725</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="120" name="Image 119"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2298700" y="135318500"/>
+          <a:ext cx="3149600" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>711</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>779142</xdr:colOff>
+      <xdr:row>712</xdr:row>
+      <xdr:rowOff>87329</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="127" name="Flèche vers la gauche 126"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19058695">
+          <a:off x="4216400" y="135534400"/>
+          <a:ext cx="690242" cy="188929"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>749300</xdr:colOff>
       <xdr:row>704</xdr:row>
@@ -7708,7 +7753,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7890,7 +7935,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8072,7 +8117,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8254,7 +8299,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8565,7 +8610,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8886,7 +8931,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9004,7 +9049,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9049,7 +9094,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9094,7 +9139,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9346,6 +9391,195 @@
           <a:ext cx="914400" cy="330200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>851</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>853</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="159" name="Ellipse 158"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7912100" y="162166300"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>574162</xdr:colOff>
+      <xdr:row>863</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>884</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="160" name="Image 159"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3050662" y="164477700"/>
+          <a:ext cx="5356737" cy="3937000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>865</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>867</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="161" name="Ellipse 160"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3098800" y="164896800"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
@@ -9721,8 +9955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A814" workbookViewId="0">
-      <selection activeCell="I845" sqref="I845"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A852" workbookViewId="0">
+      <selection activeCell="M871" sqref="M871"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Change page number fixed
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_user/screenshots.xlsx
+++ b/lisha1.00/doc_user/screenshots.xlsx
@@ -9577,6 +9577,123 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3098800" y="164896800"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>892</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>898</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="149" name="Image 148"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1282700" y="170002200"/>
+          <a:ext cx="3289300" cy="1155700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>893</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>895</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="162" name="Ellipse 161"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3556000" y="170218100"/>
           <a:ext cx="355600" cy="330200"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -9955,8 +10072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A852" workbookViewId="0">
-      <selection activeCell="M871" sqref="M871"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A876" workbookViewId="0">
+      <selection activeCell="H894" sqref="H894"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
having parsing string & load filter enhancement
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_user/screenshots.xlsx
+++ b/lisha1.00/doc_user/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="17160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -9694,6 +9694,123 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3556000" y="170218100"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>893</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>900</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="164" name="Image 163"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5969000" y="170268900"/>
+          <a:ext cx="2679700" cy="1193800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>895</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>896</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="165" name="Ellipse 164"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6807200" y="170535600"/>
           <a:ext cx="355600" cy="330200"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -10073,7 +10190,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A876" workbookViewId="0">
-      <selection activeCell="H894" sqref="H894"/>
+      <selection activeCell="K890" sqref="K890"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
New icon for record line update Documentation update
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_user/screenshots.xlsx
+++ b/lisha1.00/doc_user/screenshots.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="17480" tabRatio="500"/>
@@ -9811,6 +9811,429 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6807200" y="170535600"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>903</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>909</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="163" name="Image 162"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="172034200"/>
+          <a:ext cx="3314700" cy="1206500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>904</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>906</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="166" name="Ellipse 165"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1651000" y="172300900"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>908</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>915</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="167" name="Image 166"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId60"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5778500" y="172974000"/>
+          <a:ext cx="3022600" cy="1447800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>909</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>911</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="168" name="Ellipse 167"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7188200" y="173240700"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>922</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>929</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="169" name="Image 168"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId61"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1066800" y="175704500"/>
+          <a:ext cx="5943600" cy="1282700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>925</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>927</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="170" name="Ellipse 169"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2603500" y="176276000"/>
+          <a:ext cx="355600" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>925</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>927</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="171" name="Ellipse 170"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6375400" y="176263300"/>
           <a:ext cx="355600" cy="330200"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -10189,8 +10612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A876" workbookViewId="0">
-      <selection activeCell="K890" sqref="K890"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A908" workbookViewId="0">
+      <selection activeCell="K926" sqref="K926"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>